<commit_message>
[NEAT-40] Sync sheets (#280)
* fix; serialization of value type

* fix: Bug missing relation in conversion

* refactor; Update Alice to match david

* fix: bug creating containers without properties

* refactor; update Alice sheet

* tests: update tests

* fix: Set default view version

* tests: fix bugs and get tests to pass

* refactor: fix small bug

* refactor: default view version
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/tutorial/use-cases/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB29CD-5016-9346-9F46-A559D4A1E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545BFDE4-226C-4AD2-B78A-E0A221CA01F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>inf</t>
   </si>
   <si>
-    <t>windTurbine</t>
-  </si>
-  <si>
     <t>Inf</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>windTurbines</t>
   </si>
 </sst>
 </file>
@@ -940,46 +940,46 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="17.25" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1">
       <c r="A2" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>105</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1">
       <c r="A3" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="24"/>
@@ -1005,10 +1005,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>91</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>93</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="22">
         <v>45331</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="22">
         <v>45331</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>97</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1150,10 +1150,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>99</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>100</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>101</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>103</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -8812,22 +8812,22 @@
   </sheetPr>
   <dimension ref="A1:Z954"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1">
@@ -9420,7 +9420,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
@@ -9430,7 +9430,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="19.5" customHeight="1">
@@ -9438,7 +9438,7 @@
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -9455,7 +9455,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>21</v>
@@ -9472,7 +9472,7 @@
         <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>22</v>
@@ -9525,7 +9525,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="14" t="s">
@@ -9544,7 +9544,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="1" t="s">
@@ -9562,7 +9562,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="1" t="s">
@@ -9581,7 +9581,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="15" t="s">
@@ -9600,7 +9600,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="15" t="s">
@@ -15100,16 +15100,16 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A25"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1">

</xml_diff>

<commit_message>
feat: Added check that all classes has defined properties
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\data-modeling-lifecycle\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545BFDE4-226C-4AD2-B78A-E0A221CA01F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A971E4-86FF-4794-B281-5F3AFAFAD83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="112">
   <si>
     <t>Data model classes</t>
   </si>
@@ -344,6 +344,21 @@
   <si>
     <t>windTurbines</t>
   </si>
+  <si>
+    <t>inputVoltageLevel</t>
+  </si>
+  <si>
+    <t>outputVoltageLevel</t>
+  </si>
+  <si>
+    <t>maxCapacity</t>
+  </si>
+  <si>
+    <t>maxLevel</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
 </sst>
 </file>
 
@@ -542,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -632,6 +647,9 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8810,10 +8828,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z954"/>
+  <dimension ref="A1:Z955"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -9614,131 +9632,238 @@
       </c>
       <c r="G41" s="12"/>
     </row>
-    <row r="42" spans="1:7" ht="17.25" customHeight="1"/>
-    <row r="43" spans="1:7" ht="19.5" customHeight="1">
-      <c r="G43" s="12"/>
+    <row r="42" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="18">
+        <v>0</v>
+      </c>
+      <c r="F42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="18">
+        <v>1</v>
+      </c>
+      <c r="F43" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1">
-      <c r="C44" s="17"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="A44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="18">
+        <v>1</v>
+      </c>
+      <c r="F44" s="18">
+        <v>1</v>
+      </c>
       <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="C45" s="17"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1</v>
+      </c>
+      <c r="F45" s="12">
+        <v>1</v>
+      </c>
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>111</v>
+      </c>
       <c r="C46" s="17"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="12">
+        <v>0</v>
+      </c>
+      <c r="F46" s="12">
+        <v>1</v>
+      </c>
       <c r="G46" s="12"/>
     </row>
     <row r="47" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="C47" s="17"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="12">
+        <v>0</v>
+      </c>
+      <c r="F47" s="12">
+        <v>1</v>
+      </c>
       <c r="G47" s="12"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1">
+    <row r="48" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>111</v>
+      </c>
       <c r="C48" s="17"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="12">
+        <v>1</v>
+      </c>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="3:7" ht="15.75" customHeight="1">
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="C49" s="17"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="12">
+        <v>0</v>
+      </c>
+      <c r="F49" s="12">
+        <v>1</v>
+      </c>
       <c r="G49" s="12"/>
     </row>
-    <row r="50" spans="3:7" ht="15.75" customHeight="1">
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="C50" s="17"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
     </row>
-    <row r="51" spans="3:7" ht="15.75" customHeight="1">
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
       <c r="C51" s="17"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
     </row>
-    <row r="52" spans="3:7" ht="15.75" customHeight="1">
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
       <c r="C52" s="17"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
     </row>
-    <row r="53" spans="3:7" ht="15.75" customHeight="1">
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="C53" s="17"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
     </row>
-    <row r="54" spans="3:7" ht="15.75" customHeight="1">
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="C54" s="17"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
     </row>
-    <row r="55" spans="3:7" ht="15.75" customHeight="1">
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="C55" s="17"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
     </row>
-    <row r="56" spans="3:7" ht="15.75" customHeight="1">
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
       <c r="C56" s="17"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
     </row>
-    <row r="57" spans="3:7" ht="15.75" customHeight="1">
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
       <c r="C57" s="17"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" spans="3:7" ht="15.75" customHeight="1">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
       <c r="C58" s="17"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="3:7" ht="15.75" customHeight="1">
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="C59" s="17"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
     </row>
-    <row r="60" spans="3:7" ht="15.75" customHeight="1">
+    <row r="60" spans="1:7" ht="15.75" customHeight="1">
       <c r="C60" s="17"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
     </row>
-    <row r="61" spans="3:7" ht="15.75" customHeight="1">
+    <row r="61" spans="1:7" ht="15.75" customHeight="1">
       <c r="C61" s="17"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="3:7" ht="15.75" customHeight="1">
+    <row r="62" spans="1:7" ht="15.75" customHeight="1">
       <c r="C62" s="17"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="3:7" ht="15.75" customHeight="1">
+    <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="C63" s="17"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
     </row>
-    <row r="64" spans="3:7" ht="15.75" customHeight="1">
+    <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="C64" s="17"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -15083,6 +15208,12 @@
       <c r="E954" s="12"/>
       <c r="F954" s="12"/>
       <c r="G954" s="12"/>
+    </row>
+    <row r="955" spans="3:7" ht="15.75" customHeight="1">
+      <c r="C955" s="17"/>
+      <c r="E955" s="12"/>
+      <c r="F955" s="12"/>
+      <c r="G955" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -15099,8 +15230,8 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
changed matchtype to match for info rules
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/data-modeling-lifecycle/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C96AEE6-0603-4249-B4DF-EF9BC2A9F56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B300B57-3C62-1949-8202-BEFF258387BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="2800" windowWidth="27380" windowHeight="23940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="112">
   <si>
     <t>Data model classes</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>Max Count</t>
-  </si>
-  <si>
-    <t>MatchType</t>
   </si>
   <si>
     <t>name</t>
@@ -691,15 +688,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -709,13 +697,7 @@
     <xf numFmtId="3" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -740,6 +722,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1055,9 +1052,7 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView zoomScale="254" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView zoomScale="254" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1075,26 +1070,26 @@
   <sheetData>
     <row r="1" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -1120,10 +1115,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>89</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1149,10 +1144,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1178,10 +1173,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1207,10 +1202,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1236,7 +1231,7 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="10">
         <v>45331</v>
@@ -1265,7 +1260,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="10">
         <v>45331</v>
@@ -1294,10 +1289,10 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1323,10 +1318,10 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -8930,8 +8925,8 @@
   </sheetPr>
   <dimension ref="A1:U962"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8949,16 +8944,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="A1" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -8974,29 +8969,29 @@
       <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="38" t="s">
-        <v>38</v>
+      <c r="H2" s="35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9004,11 +8999,11 @@
         <v>6</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="24">
         <v>1</v>
@@ -9024,11 +9019,11 @@
         <v>6</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="24">
         <v>1</v>
@@ -9044,11 +9039,11 @@
         <v>6</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="24">
         <v>1</v>
@@ -9064,7 +9059,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23" t="s">
@@ -9077,7 +9072,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>8</v>
@@ -9088,11 +9083,11 @@
         <v>9</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="28">
         <v>0</v>
@@ -9108,11 +9103,11 @@
         <v>9</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="28">
         <v>1</v>
@@ -9128,11 +9123,11 @@
         <v>9</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="28">
         <v>1</v>
@@ -9148,7 +9143,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27" t="s">
@@ -9168,11 +9163,11 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="28">
         <v>0</v>
@@ -9188,11 +9183,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="24">
         <v>1</v>
@@ -9208,7 +9203,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
@@ -9228,11 +9223,11 @@
         <v>11</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="24">
         <v>1</v>
@@ -9248,11 +9243,11 @@
         <v>11</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="24">
         <v>1</v>
@@ -9268,7 +9263,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
@@ -9277,8 +9272,8 @@
       <c r="E16" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="47" t="s">
-        <v>70</v>
+      <c r="F16" s="42" t="s">
+        <v>69</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
@@ -9288,7 +9283,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="27" t="s">
@@ -9308,7 +9303,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="27" t="s">
@@ -9317,8 +9312,8 @@
       <c r="E18" s="28">
         <v>1</v>
       </c>
-      <c r="F18" s="47" t="s">
-        <v>69</v>
+      <c r="F18" s="42" t="s">
+        <v>68</v>
       </c>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
@@ -9328,7 +9323,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="27" t="s">
@@ -9348,11 +9343,11 @@
         <v>20</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="24">
         <v>1</v>
@@ -9368,7 +9363,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="23" t="s">
@@ -9388,11 +9383,11 @@
         <v>20</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="24">
         <v>1</v>
@@ -9408,11 +9403,11 @@
         <v>20</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="24">
         <v>0</v>
@@ -9428,11 +9423,11 @@
         <v>16</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="28">
         <v>1</v>
@@ -9448,11 +9443,11 @@
         <v>16</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="28">
         <v>0</v>
@@ -9468,11 +9463,11 @@
         <v>16</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="28">
         <v>2</v>
@@ -9488,11 +9483,11 @@
         <v>16</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" s="28">
         <v>2</v>
@@ -9508,11 +9503,11 @@
         <v>16</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" s="28">
         <v>2</v>
@@ -9528,11 +9523,11 @@
         <v>16</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="28">
         <v>1</v>
@@ -9548,7 +9543,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="27" t="s">
@@ -9568,7 +9563,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="27" t="s">
@@ -9588,11 +9583,11 @@
         <v>16</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="28">
         <v>1</v>
@@ -9608,11 +9603,11 @@
         <v>16</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" s="28">
         <v>1</v>
@@ -9628,7 +9623,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="23" t="s">
@@ -9638,7 +9633,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
@@ -9648,7 +9643,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="23" t="s">
@@ -9665,10 +9660,10 @@
     </row>
     <row r="36" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="23" t="s">
@@ -9685,10 +9680,10 @@
     </row>
     <row r="37" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="27" t="s">
@@ -9708,7 +9703,7 @@
         <v>19</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="27" t="s">
@@ -9728,31 +9723,31 @@
         <v>19</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E39" s="28">
         <v>1</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
     </row>
     <row r="40" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" s="24">
         <v>1</v>
@@ -9765,34 +9760,34 @@
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>109</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>110</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E41" s="24">
         <v>1</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G41" s="25"/>
       <c r="H41" s="25"/>
     </row>
     <row r="42" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="24">
         <v>1</v>
@@ -9808,11 +9803,11 @@
         <v>24</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E43" s="28">
         <v>1</v>
@@ -9828,7 +9823,7 @@
         <v>24</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="27" t="s">
@@ -9848,11 +9843,11 @@
         <v>24</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E45" s="28">
         <v>1</v>
@@ -9867,32 +9862,32 @@
       <c r="A46" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="50">
+      <c r="E46" s="45">
         <v>1</v>
       </c>
-      <c r="F46" s="50">
+      <c r="F46" s="45">
         <v>1</v>
       </c>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
     </row>
     <row r="47" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="24">
         <v>1</v>
@@ -9908,11 +9903,11 @@
         <v>28</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" s="24">
         <v>1</v>
@@ -9928,7 +9923,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27" t="s">
@@ -9938,7 +9933,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G49" s="29"/>
       <c r="H49" s="29"/>
@@ -9948,7 +9943,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="23" t="s">
@@ -9958,21 +9953,21 @@
         <v>3</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" s="29"/>
       <c r="D51" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E51" s="32">
         <v>0</v>
@@ -9985,14 +9980,14 @@
     </row>
     <row r="52" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="25"/>
       <c r="D52" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E52" s="33">
         <v>1</v>
@@ -10005,14 +10000,14 @@
     </row>
     <row r="53" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" s="25"/>
       <c r="D53" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E53" s="33">
         <v>1</v>
@@ -10025,14 +10020,14 @@
     </row>
     <row r="54" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="34"/>
       <c r="D54" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E54" s="28">
         <v>1</v>
@@ -10045,14 +10040,14 @@
     </row>
     <row r="55" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" s="34"/>
       <c r="D55" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E55" s="28">
         <v>0</v>
@@ -10065,14 +10060,14 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C56" s="34"/>
       <c r="D56" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E56" s="28">
         <v>0</v>
@@ -14630,7 +14625,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A28" sqref="A4:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14643,13 +14638,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -14673,19 +14668,19 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -14710,7 +14705,7 @@
       <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="39" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="19" t="s">
@@ -14736,7 +14731,7 @@
       <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="19" t="s">
@@ -14787,7 +14782,7 @@
     </row>
     <row r="11" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="19" t="s">
@@ -14835,29 +14830,29 @@
       <c r="C15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="46" t="s">
-        <v>105</v>
+      <c r="D15" s="41" t="s">
+        <v>104</v>
       </c>
       <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="19"/>
-      <c r="D17" s="46"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14873,7 +14868,7 @@
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="19" t="s">
@@ -14907,7 +14902,7 @@
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="38" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="19"/>
@@ -14934,7 +14929,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -14943,7 +14938,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -14952,7 +14947,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -14961,7 +14956,7 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -14970,7 +14965,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
@@ -15957,5 +15952,6 @@
     <hyperlink ref="D15" r:id="rId3" location="ACLineSegment" xr:uid="{F4B5E2F6-DECF-D34E-BEDF-4A8FE9E313DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed to match type for info rules
</commit_message>
<xml_diff>
--- a/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
+++ b/docs/data-modeling-lifecycle/spreadsheets/information-architect-david.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/data-modeling-lifecycle/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B300B57-3C62-1949-8202-BEFF258387BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F3202E-7E0E-254E-AFB9-6253753E6668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="2800" windowWidth="27380" windowHeight="23940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <t>Match</t>
   </si>
   <si>
     <t>GeneratingUnit</t>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>consumption</t>
+  </si>
+  <si>
+    <t>Match Type</t>
   </si>
 </sst>
 </file>
@@ -1070,26 +1070,26 @@
   <sheetData>
     <row r="1" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1144,10 +1144,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1173,10 +1173,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="10">
         <v>45331</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="10">
         <v>45331</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -8925,8 +8925,8 @@
   </sheetPr>
   <dimension ref="A1:U962"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8945,7 +8945,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -8973,37 +8973,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="37" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>37</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="24">
         <v>1</v>
@@ -9016,14 +9016,14 @@
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="24">
         <v>1</v>
@@ -9036,14 +9036,14 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="24">
         <v>1</v>
@@ -9056,14 +9056,14 @@
     </row>
     <row r="6" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="24">
         <v>1</v>
@@ -9072,22 +9072,22 @@
         <v>1</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="28">
         <v>0</v>
@@ -9100,14 +9100,14 @@
     </row>
     <row r="8" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="28">
         <v>1</v>
@@ -9120,14 +9120,14 @@
     </row>
     <row r="9" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="28">
         <v>1</v>
@@ -9140,14 +9140,14 @@
     </row>
     <row r="10" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -9160,14 +9160,14 @@
     </row>
     <row r="11" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="28">
         <v>0</v>
@@ -9180,14 +9180,14 @@
     </row>
     <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="24">
         <v>1</v>
@@ -9200,14 +9200,14 @@
     </row>
     <row r="13" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="24">
         <v>0</v>
@@ -9220,14 +9220,14 @@
     </row>
     <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="24">
         <v>1</v>
@@ -9240,14 +9240,14 @@
     </row>
     <row r="15" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="24">
         <v>1</v>
@@ -9260,34 +9260,34 @@
     </row>
     <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="28">
         <v>1</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="28">
         <v>1</v>
@@ -9300,34 +9300,34 @@
     </row>
     <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="28">
         <v>1</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="28">
         <v>1</v>
@@ -9340,14 +9340,14 @@
     </row>
     <row r="20" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="24">
         <v>1</v>
@@ -9360,14 +9360,14 @@
     </row>
     <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" s="24">
         <v>1</v>
@@ -9380,14 +9380,14 @@
     </row>
     <row r="22" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="24">
         <v>1</v>
@@ -9400,14 +9400,14 @@
     </row>
     <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="24">
         <v>0</v>
@@ -9420,14 +9420,14 @@
     </row>
     <row r="24" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E24" s="28">
         <v>1</v>
@@ -9440,14 +9440,14 @@
     </row>
     <row r="25" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="28">
         <v>0</v>
@@ -9460,14 +9460,14 @@
     </row>
     <row r="26" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="28">
         <v>2</v>
@@ -9480,14 +9480,14 @@
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="28">
         <v>2</v>
@@ -9500,14 +9500,14 @@
     </row>
     <row r="28" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" s="28">
         <v>2</v>
@@ -9520,14 +9520,14 @@
     </row>
     <row r="29" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E29" s="28">
         <v>1</v>
@@ -9540,14 +9540,14 @@
     </row>
     <row r="30" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" s="28">
         <v>1</v>
@@ -9560,14 +9560,14 @@
     </row>
     <row r="31" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" s="28">
         <v>1</v>
@@ -9580,14 +9580,14 @@
     </row>
     <row r="32" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="28">
         <v>1</v>
@@ -9600,14 +9600,14 @@
     </row>
     <row r="33" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" s="28">
         <v>1</v>
@@ -9620,34 +9620,34 @@
     </row>
     <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="24">
         <v>1</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="24">
         <v>1</v>
@@ -9660,14 +9660,14 @@
     </row>
     <row r="36" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" s="24">
         <v>1</v>
@@ -9680,14 +9680,14 @@
     </row>
     <row r="37" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" s="28">
         <v>1</v>
@@ -9700,14 +9700,14 @@
     </row>
     <row r="38" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" s="28">
         <v>1</v>
@@ -9720,34 +9720,34 @@
     </row>
     <row r="39" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E39" s="28">
         <v>1</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
     </row>
     <row r="40" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E40" s="24">
         <v>1</v>
@@ -9760,34 +9760,34 @@
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>108</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>109</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E41" s="24">
         <v>1</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G41" s="25"/>
       <c r="H41" s="25"/>
     </row>
     <row r="42" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E42" s="24">
         <v>1</v>
@@ -9800,14 +9800,14 @@
     </row>
     <row r="43" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="28">
         <v>1</v>
@@ -9820,14 +9820,14 @@
     </row>
     <row r="44" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="27"/>
       <c r="D44" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E44" s="28">
         <v>1</v>
@@ -9840,14 +9840,14 @@
     </row>
     <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E45" s="28">
         <v>1</v>
@@ -9860,14 +9860,14 @@
     </row>
     <row r="46" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="44"/>
       <c r="D46" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" s="45">
         <v>1</v>
@@ -9880,14 +9880,14 @@
     </row>
     <row r="47" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="31"/>
       <c r="D47" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E47" s="24">
         <v>1</v>
@@ -9900,14 +9900,14 @@
     </row>
     <row r="48" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" s="24">
         <v>1</v>
@@ -9920,54 +9920,54 @@
     </row>
     <row r="49" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E49" s="28">
         <v>2</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="29"/>
       <c r="H49" s="29"/>
     </row>
     <row r="50" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E50" s="24">
         <v>3</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="29"/>
       <c r="D51" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" s="32">
         <v>0</v>
@@ -9980,14 +9980,14 @@
     </row>
     <row r="52" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="25"/>
       <c r="D52" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E52" s="33">
         <v>1</v>
@@ -10000,14 +10000,14 @@
     </row>
     <row r="53" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="25"/>
       <c r="D53" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E53" s="33">
         <v>1</v>
@@ -10020,14 +10020,14 @@
     </row>
     <row r="54" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54" s="34"/>
       <c r="D54" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E54" s="28">
         <v>1</v>
@@ -10040,14 +10040,14 @@
     </row>
     <row r="55" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" s="34"/>
       <c r="D55" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E55" s="28">
         <v>0</v>
@@ -10060,14 +10060,14 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C56" s="34"/>
       <c r="D56" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E56" s="28">
         <v>0</v>
@@ -14624,8 +14624,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="A28" sqref="A4:A28"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14634,7 +14634,8 @@
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14681,66 +14682,66 @@
         <v>4</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="19"/>
       <c r="D3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
       <c r="D5" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -14749,51 +14750,51 @@
     </row>
     <row r="8" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -14802,53 +14803,53 @@
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="19"/>
@@ -14857,79 +14858,79 @@
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -14938,7 +14939,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -14947,7 +14948,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -14956,7 +14957,7 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
@@ -14965,7 +14966,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>

</xml_diff>